<commit_message>
put Xspress3 IOC on SCI network, EPICS tagged
</commit_message>
<xml_diff>
--- a/current.xlsx
+++ b/current.xlsx
@@ -19,8 +19,33 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>BR</author>
+  </authors>
+  <commentList>
+    <comment ref="A8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Why are these two (Pilatus) occupying precious POE ports?
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="309">
   <si>
     <t xml:space="preserve">Switch</t>
   </si>
@@ -133,7 +158,7 @@
     <t xml:space="preserve">10.68.40.29</t>
   </si>
   <si>
-    <t xml:space="preserve">why is this mac showing up?</t>
+    <t xml:space="preserve">second Pilatus interface, should be xf06bm-Pilatus-data?</t>
   </si>
   <si>
     <t xml:space="preserve">1/1/6</t>
@@ -775,7 +800,10 @@
     <t xml:space="preserve">xf06bm-ioc-xspress3</t>
   </si>
   <si>
-    <t xml:space="preserve">10.68.43.31</t>
+    <t xml:space="preserve">10.68.40.31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tagged for EPICS vlan, 10.68.43.31</t>
   </si>
   <si>
     <t xml:space="preserve">6</t>
@@ -1150,23 +1178,23 @@
   </sheetPr>
   <dimension ref="A1:K167"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J72" activeCellId="0" sqref="J72"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K125" activeCellId="0" sqref="K125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="49.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4945,13 +4973,16 @@
       <c r="J124" s="3" t="s">
         <v>251</v>
       </c>
+      <c r="K124" s="0" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="3" t="s">
         <v>242</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C125" s="3" t="s">
         <v>67</v>
@@ -4981,7 +5012,7 @@
         <v>242</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>67</v>
@@ -5011,7 +5042,7 @@
         <v>242</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>67</v>
@@ -5041,7 +5072,7 @@
         <v>242</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>67</v>
@@ -5071,7 +5102,7 @@
         <v>242</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>67</v>
@@ -5101,7 +5132,7 @@
         <v>242</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>67</v>
@@ -5131,7 +5162,7 @@
         <v>242</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>248</v>
@@ -5149,13 +5180,13 @@
         <v>650</v>
       </c>
       <c r="H131" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I131" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="J131" s="3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5163,7 +5194,7 @@
         <v>242</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>248</v>
@@ -5181,13 +5212,13 @@
         <v>650</v>
       </c>
       <c r="H132" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="I132" s="3" t="s">
         <v>166</v>
       </c>
       <c r="J132" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5195,7 +5226,7 @@
         <v>242</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>67</v>
@@ -5225,7 +5256,7 @@
         <v>242</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C134" s="3" t="s">
         <v>67</v>
@@ -5255,7 +5286,7 @@
         <v>242</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C135" s="3" t="s">
         <v>67</v>
@@ -5285,7 +5316,7 @@
         <v>242</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>67</v>
@@ -5315,7 +5346,7 @@
         <v>242</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>67</v>
@@ -5345,7 +5376,7 @@
         <v>242</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C138" s="3" t="s">
         <v>67</v>
@@ -5375,7 +5406,7 @@
         <v>242</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C139" s="3" t="s">
         <v>67</v>
@@ -5405,7 +5436,7 @@
         <v>242</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C140" s="3" t="s">
         <v>67</v>
@@ -5435,7 +5466,7 @@
         <v>242</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C141" s="3" t="s">
         <v>67</v>
@@ -5465,7 +5496,7 @@
         <v>242</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C142" s="3" t="s">
         <v>67</v>
@@ -5495,7 +5526,7 @@
         <v>242</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C143" s="3" t="s">
         <v>67</v>
@@ -5525,7 +5556,7 @@
         <v>242</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C144" s="3" t="s">
         <v>67</v>
@@ -5555,7 +5586,7 @@
         <v>242</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C145" s="3" t="s">
         <v>67</v>
@@ -5585,7 +5616,7 @@
         <v>242</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C146" s="3" t="s">
         <v>67</v>
@@ -5615,7 +5646,7 @@
         <v>242</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>67</v>
@@ -5645,7 +5676,7 @@
         <v>242</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C148" s="3" t="s">
         <v>67</v>
@@ -5675,7 +5706,7 @@
         <v>242</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C149" s="3" t="s">
         <v>67</v>
@@ -5705,7 +5736,7 @@
         <v>242</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C150" s="3" t="s">
         <v>248</v>
@@ -5723,13 +5754,13 @@
         <v>652</v>
       </c>
       <c r="H150" s="3" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I150" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="J150" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5737,7 +5768,7 @@
         <v>242</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C151" s="3" t="s">
         <v>67</v>
@@ -5767,7 +5798,7 @@
         <v>242</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C152" s="3" t="s">
         <v>67</v>
@@ -5797,7 +5828,7 @@
         <v>242</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C153" s="3" t="s">
         <v>67</v>
@@ -5827,7 +5858,7 @@
         <v>242</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>67</v>
@@ -5857,7 +5888,7 @@
         <v>242</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C155" s="3" t="s">
         <v>67</v>
@@ -5887,7 +5918,7 @@
         <v>242</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>67</v>
@@ -5917,7 +5948,7 @@
         <v>242</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C157" s="3" t="s">
         <v>67</v>
@@ -5947,7 +5978,7 @@
         <v>242</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C158" s="3" t="s">
         <v>67</v>
@@ -5977,7 +6008,7 @@
         <v>242</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C159" s="3" t="s">
         <v>67</v>
@@ -6007,7 +6038,7 @@
         <v>242</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C160" s="3" t="s">
         <v>67</v>
@@ -6037,7 +6068,7 @@
         <v>242</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C161" s="3" t="s">
         <v>67</v>
@@ -6067,7 +6098,7 @@
         <v>242</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C162" s="3" t="s">
         <v>67</v>
@@ -6088,10 +6119,10 @@
         <v>58</v>
       </c>
       <c r="I162" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J162" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6099,7 +6130,7 @@
         <v>242</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C163" s="3" t="s">
         <v>67</v>
@@ -6120,10 +6151,10 @@
         <v>58</v>
       </c>
       <c r="I163" s="5" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="J163" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6131,7 +6162,7 @@
         <v>242</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C164" s="3" t="s">
         <v>67</v>
@@ -6152,10 +6183,10 @@
         <v>58</v>
       </c>
       <c r="I164" s="5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="J164" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6163,7 +6194,7 @@
         <v>242</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C165" s="3" t="s">
         <v>67</v>
@@ -6184,10 +6215,10 @@
         <v>58</v>
       </c>
       <c r="I165" s="5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="J165" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6195,7 +6226,7 @@
         <v>242</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C166" s="3" t="s">
         <v>67</v>
@@ -6225,7 +6256,7 @@
         <v>242</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C167" s="3" t="s">
         <v>67</v>
@@ -6253,11 +6284,12 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update entry for pilatus
</commit_message>
<xml_diff>
--- a/current.xlsx
+++ b/current.xlsx
@@ -158,7 +158,7 @@
     <t xml:space="preserve">10.68.40.29</t>
   </si>
   <si>
-    <t xml:space="preserve">second Pilatus interface, should be xf06bm-Pilatus-data?</t>
+    <t xml:space="preserve">pre-reIP second Pilatus interface, should not be active</t>
   </si>
   <si>
     <t xml:space="preserve">1/1/6</t>
@@ -1266,11 +1266,11 @@
   </sheetPr>
   <dimension ref="A1:K167"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A134" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I154" activeCellId="0" sqref="I154"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.66"/>

</xml_diff>